<commit_message>
Update check list and database
</commit_message>
<xml_diff>
--- a/document/tasksheet/TaskAll.xlsx
+++ b/document/tasksheet/TaskAll.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>Report</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Document  + Report + Meeting Report+ dựng mô hình</t>
+  </si>
+  <si>
+    <t>Nhận Module cc1310</t>
+  </si>
+  <si>
+    <t>26/05/2016</t>
+  </si>
+  <si>
+    <t>Cảm biến Nhiêt độ độ ẩm AM2320</t>
   </si>
 </sst>
 </file>
@@ -799,15 +808,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
@@ -1170,6 +1180,22 @@
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E2:H2"/>

</xml_diff>